<commit_message>
to do pdf file
</commit_message>
<xml_diff>
--- a/List of todo .xlsx
+++ b/List of todo .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jschandra/dev/book_bag_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92C4357C-B67A-5346-8D33-FBF3B2A54131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C9702F3-2786-674D-82AC-E423F1C1AEB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{C6F53C86-E03E-1745-8BE1-03570E22C3B4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Code Lines</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>Student can only borrow if book is available, and if the book is in his/her book bag, the borrow button should disappear</t>
+  </si>
+  <si>
+    <t>Added if/else/else if conditional statements in the ejs file but does not seem to work when the book is in the book bag and when quantity is 0</t>
+  </si>
+  <si>
+    <t>javascript if/else/else if functions</t>
+  </si>
+  <si>
+    <t>views/users/mainStudent.ejs,</t>
   </si>
 </sst>
 </file>
@@ -738,32 +750,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFAFFAA5-9DA8-AD4A-93D2-7101C0FF047D}">
-  <dimension ref="A1:J20"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" customWidth="1"/>
-    <col min="4" max="4" width="84" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" customWidth="1"/>
     <col min="7" max="7" width="24.5" customWidth="1"/>
-    <col min="8" max="8" width="47.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
     <col min="9" max="9" width="33" customWidth="1"/>
     <col min="10" max="10" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="5">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="5">
         <f ca="1">NOW()</f>
-        <v>43779.44493391204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+        <v>43779.450549768517</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
@@ -792,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="110" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" s="1" customFormat="1" ht="264" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -821,9 +837,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" s="1" customFormat="1" ht="110" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="2:10" s="1" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -838,9 +877,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="154" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" s="1" customFormat="1" ht="154" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
@@ -865,9 +904,9 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="88" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" s="1" customFormat="1" ht="88" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -886,9 +925,9 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="176" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" s="1" customFormat="1" ht="176" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>29</v>
@@ -905,7 +944,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -915,7 +954,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -925,7 +964,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -935,7 +974,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -945,7 +984,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -955,7 +994,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -965,7 +1004,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" s="1" customFormat="1" ht="73" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1017,6 +1056,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="44" fitToHeight="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
with changes from Kenny
</commit_message>
<xml_diff>
--- a/List of todo .xlsx
+++ b/List of todo .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jschandra/dev/book_bag_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C9702F3-2786-674D-82AC-E423F1C1AEB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7280714A-35E1-874E-995F-CD2CDBF71EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{C6F53C86-E03E-1745-8BE1-03570E22C3B4}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{C6F53C86-E03E-1745-8BE1-03570E22C3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -776,7 +776,7 @@
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" s="5">
         <f ca="1">NOW()</f>
-        <v>43779.450549768517</v>
+        <v>43781.371100925928</v>
       </c>
     </row>
     <row r="3" spans="2:10" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">

</xml_diff>